<commit_message>
App for uploading excel sensor data and displaying/graphing
</commit_message>
<xml_diff>
--- a/mysite/temperature_data.xlsx
+++ b/mysite/temperature_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary\Documents\swproject\mysite\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -131,7 +131,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>User 1</a:t>
+              <a:t>Sensor Data vs Time</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2047,11 +2047,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-586458896"/>
-        <c:axId val="-586467056"/>
+        <c:axId val="437734320"/>
+        <c:axId val="437728336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-586458896"/>
+        <c:axId val="437734320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2150,7 +2150,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-586467056"/>
+        <c:crossAx val="437728336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2158,7 +2158,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-586467056"/>
+        <c:axId val="437728336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2265,7 +2265,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-586458896"/>
+        <c:crossAx val="437734320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4301,11 +4301,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-269620672"/>
-        <c:axId val="-269620128"/>
+        <c:axId val="437735952"/>
+        <c:axId val="437736496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-269620672"/>
+        <c:axId val="437735952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4404,7 +4404,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-269620128"/>
+        <c:crossAx val="437736496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4412,7 +4412,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-269620128"/>
+        <c:axId val="437736496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4519,7 +4519,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-269620672"/>
+        <c:crossAx val="437735952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6551,11 +6551,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-269619584"/>
-        <c:axId val="-269629376"/>
+        <c:axId val="437722896"/>
+        <c:axId val="437728880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-269619584"/>
+        <c:axId val="437722896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6654,7 +6654,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-269629376"/>
+        <c:crossAx val="437728880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6662,7 +6662,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-269629376"/>
+        <c:axId val="437728880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6773,7 +6773,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-269619584"/>
+        <c:crossAx val="437722896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8893,7 +8893,7 @@
   <dimension ref="A1:D99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>